<commit_message>
76x35 sent to fab house
</commit_message>
<xml_diff>
--- a/hardware/plug/1v2/Enclosure/0v4_Alu_Sample_76x35/BOM_76x35.xlsx
+++ b/hardware/plug/1v2/Enclosure/0v4_Alu_Sample_76x35/BOM_76x35.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Borec\Documents\GitHub\LimeSDR-USB\hardware\plug\1v2\Enclosure\0v3_Alu_Sample_better_documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Borec\Documents\GitHub\LimeSDR-USB\hardware\plug\1v2\Enclosure\0v4_Alu_Sample_76x35\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
   <si>
     <t>-----------------------------------</t>
   </si>
@@ -81,33 +81,18 @@
     <t>http://dangerousprototypes.com/store/pcbs</t>
   </si>
   <si>
-    <t>TaoBao?</t>
-  </si>
-  <si>
-    <t>http://www.ebay.com/itm/121992475879?var=420993987775</t>
-  </si>
-  <si>
     <t>http://www.ebay.com/itm/141938770196?var=441070380530</t>
   </si>
   <si>
     <t>http://www.ebay.com/itm/281744593873?var=580748876938</t>
   </si>
   <si>
-    <t>combined in China and shipped to World</t>
-  </si>
-  <si>
-    <t>expected price</t>
-  </si>
-  <si>
     <t>4x M3 nuts</t>
   </si>
   <si>
     <t>http://www.ebay.com/itm/301833214296?var=600643443952</t>
   </si>
   <si>
-    <t>8x M3x10 SS Button Head Socket Cap Screw</t>
-  </si>
-  <si>
     <t>http://www.ebay.com/itm/121992475879?var=420993987756</t>
   </si>
   <si>
@@ -118,13 +103,19 @@
   </si>
   <si>
     <t>http://www.ebay.com/itm/381492683443</t>
+  </si>
+  <si>
+    <t>8x M2.5x12 SS Button Head Socket Cap Screw</t>
+  </si>
+  <si>
+    <t>http://www.ebay.com/itm/122045959948?var=421066267740</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,14 +128,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -175,16 +158,8 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="16"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -194,11 +169,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
     <fill>
@@ -231,38 +201,33 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="4">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
-    <cellStyle name="Good" xfId="2" builtinId="26"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
-    <cellStyle name="Neutral" xfId="4" builtinId="28"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -541,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5:E19"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,19 +519,19 @@
     <col min="3" max="3" width="21.140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="28.140625" customWidth="1"/>
     <col min="5" max="5" width="31.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="5" t="s">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="B1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" s="6"/>
-    </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C1" s="6"/>
+    </row>
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -576,72 +541,66 @@
       <c r="C2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
       <c r="C4"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C5">
         <v>4.99</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C6">
         <f>3.99/100*4</f>
         <v>0.15960000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C7">
         <f>3.69/100*4</f>
         <v>0.14760000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>28</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C8">
-        <f>4.39/100*8</f>
-        <v>0.35119999999999996</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <f>4/100*8</f>
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -653,7 +612,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -665,50 +624,50 @@
         <v>7.9600000000000004E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="5">
         <v>14.63</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C12"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
       <c r="C13"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>5</v>
       </c>
       <c r="C14"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
       <c r="C15"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>6</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C16">
         <v>1.2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -719,18 +678,18 @@
         <v>1.76</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>8</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C18">
         <v>1.51</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -741,65 +700,51 @@
         <v>1.85</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="C21" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E21" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C22">
         <f>SUM(C5:C11)</f>
-        <v>22.957999999999998</v>
-      </c>
-      <c r="E22">
-        <f>SUM(E5:E11)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>22.9268</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C23"/>
     </row>
-    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="C24" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E24" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C25">
         <f>SUM(C22,C16:C19)</f>
-        <v>29.278000000000002</v>
-      </c>
-      <c r="E25">
-        <f>SUM(E22,E16:E19)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>29.246800000000004</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C26"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C27"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C28"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
       <c r="C29"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C30"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C31"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C32"/>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.25">
@@ -815,9 +760,8 @@
       <c r="C36"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B17" r:id="rId1"/>

</xml_diff>

<commit_message>
quick change: readme, bom
</commit_message>
<xml_diff>
--- a/hardware/plug/1v2/Enclosure/0v4_Alu_Sample_76x35/BOM_76x35.xlsx
+++ b/hardware/plug/1v2/Enclosure/0v4_Alu_Sample_76x35/BOM_76x35.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>-----------------------------------</t>
   </si>
@@ -27,9 +27,6 @@
     <t>material:</t>
   </si>
   <si>
-    <t>1x PCB panel 10x10 cm (Front panel, rear panel, 4x holders)</t>
-  </si>
-  <si>
     <t>4 rubber pads</t>
   </si>
   <si>
@@ -51,9 +48,6 @@
     <t>wire cutters for removing breaktabs</t>
   </si>
   <si>
-    <t>for prototype</t>
-  </si>
-  <si>
     <t>http://www.ebay.com/itm/121948184468</t>
   </si>
   <si>
@@ -69,15 +63,6 @@
     <t>http://www.ebay.com/itm/361356150996</t>
   </si>
   <si>
-    <t>price (USD) includes shipping to Europe</t>
-  </si>
-  <si>
-    <t>combined with tools (shipping included):</t>
-  </si>
-  <si>
-    <t>combined, no tools (shipping included):</t>
-  </si>
-  <si>
     <t>http://dangerousprototypes.com/store/pcbs</t>
   </si>
   <si>
@@ -109,25 +94,25 @@
   </si>
   <si>
     <t>http://www.ebay.com/itm/122045959948?var=421066267740</t>
+  </si>
+  <si>
+    <t>(if not present) 3.5 x 1.35mm DC jack socket Female for PCB</t>
+  </si>
+  <si>
+    <t>http://www.ebay.com/itm/271542964705</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1x PCB panel 10x10 cm (Front panel, rear panel, 4x holders) for 10pcs </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -142,42 +127,16 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -185,49 +144,24 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="4">
-    <cellStyle name="Calculation" xfId="1" builtinId="22"/>
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
-    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -506,15 +440,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="54.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="63.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="55.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="28.140625" customWidth="1"/>
@@ -525,21 +459,15 @@
     <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="6"/>
-    </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C1"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -555,10 +483,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>27</v>
+        <v>21</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="C5">
         <v>4.99</v>
@@ -566,10 +494,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C6">
         <f>3.99/100*4</f>
@@ -578,10 +506,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C7">
         <f>3.69/100*4</f>
@@ -590,10 +518,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C8">
         <f>4/100*8</f>
@@ -602,22 +530,22 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C9">
-        <f>26/10</f>
-        <v>2.6</v>
+        <f>26</f>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C10">
         <f>1.99/100*4</f>
@@ -625,105 +553,106 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>4</v>
+      <c r="A11" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="5">
+        <v>12</v>
+      </c>
+      <c r="C11" s="4">
         <v>14.63</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C12"/>
+      <c r="A12" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12">
+        <f>2/10</f>
+        <v>0.2</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>0</v>
-      </c>
+      <c r="A13" s="4"/>
+      <c r="B13" s="1"/>
       <c r="C13"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C14"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C15"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16">
-        <v>1.2</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="C16"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C17">
-        <v>1.76</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C18">
-        <v>1.51</v>
+        <v>1.76</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C19">
+        <v>1.51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20">
         <v>1.85</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="C21" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C22">
-        <f>SUM(C5:C11)</f>
-        <v>22.9268</v>
-      </c>
+      <c r="C22"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C23"/>
     </row>
-    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="C24" s="3" t="s">
-        <v>17</v>
-      </c>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C24"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C25">
-        <f>SUM(C22,C16:C19)</f>
-        <v>29.246800000000004</v>
-      </c>
+      <c r="C25"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C26"/>
@@ -735,10 +664,10 @@
       <c r="C28"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B29" s="1"/>
       <c r="C29"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="1"/>
       <c r="C30"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -759,23 +688,24 @@
     <row r="36" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C36"/>
     </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C37"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:C1"/>
-  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B17" r:id="rId1"/>
-    <hyperlink ref="B19" r:id="rId2"/>
+    <hyperlink ref="B18" r:id="rId1"/>
+    <hyperlink ref="B20" r:id="rId2"/>
     <hyperlink ref="B11" r:id="rId3"/>
     <hyperlink ref="B10" r:id="rId4"/>
     <hyperlink ref="B9" r:id="rId5"/>
-    <hyperlink ref="B18" r:id="rId6"/>
+    <hyperlink ref="B19" r:id="rId6"/>
     <hyperlink ref="B6" r:id="rId7"/>
     <hyperlink ref="B8" r:id="rId8"/>
-    <hyperlink ref="B16" r:id="rId9"/>
+    <hyperlink ref="B17" r:id="rId9"/>
     <hyperlink ref="B5" r:id="rId10"/>
+    <hyperlink ref="B12" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId11"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
BOM comments and screws are (optional)
</commit_message>
<xml_diff>
--- a/hardware/plug/1v2/Enclosure/0v4_Alu_Sample_76x35/BOM_76x35.xlsx
+++ b/hardware/plug/1v2/Enclosure/0v4_Alu_Sample_76x35/BOM_76x35.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t>-----------------------------------</t>
   </si>
@@ -27,9 +27,6 @@
     <t>material:</t>
   </si>
   <si>
-    <t>4 rubber pads</t>
-  </si>
-  <si>
     <t>11x 5cm SMA to U.fl cables</t>
   </si>
   <si>
@@ -90,19 +87,31 @@
     <t>http://www.ebay.com/itm/381492683443</t>
   </si>
   <si>
-    <t>8x M2.5x12 SS Button Head Socket Cap Screw</t>
-  </si>
-  <si>
     <t>http://www.ebay.com/itm/122045959948?var=421066267740</t>
   </si>
   <si>
-    <t>(if not present) 3.5 x 1.35mm DC jack socket Female for PCB</t>
-  </si>
-  <si>
     <t>http://www.ebay.com/itm/271542964705</t>
   </si>
   <si>
     <t xml:space="preserve">PCB panel 10x10 cm (Front panel, rear panel, 4x holders) for 10pcs </t>
+  </si>
+  <si>
+    <t>4 rubber pads/feet</t>
+  </si>
+  <si>
+    <t>(optional) 3.5 x 1.35mm DC jack socket Female for PCB</t>
+  </si>
+  <si>
+    <t>(optional) 8x M2.5x12 SS Button Head Socket Cap Screw</t>
+  </si>
+  <si>
+    <t>REMARK</t>
+  </si>
+  <si>
+    <t>if not yet populated on board, have seen some proto board without</t>
+  </si>
+  <si>
+    <t>phillips head screws included with enclosure, I prefer hex allen key screws</t>
   </si>
 </sst>
 </file>
@@ -149,7 +158,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -159,6 +168,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -440,17 +451,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="63.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="60.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="55.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11" style="2" customWidth="1"/>
     <col min="4" max="4" width="28.140625" customWidth="1"/>
     <col min="5" max="5" width="31.5703125" customWidth="1"/>
     <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
@@ -459,191 +470,202 @@
     <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C4"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="C5">
         <v>4.99</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="C6">
         <f>3.99/100*4</f>
         <v>0.15960000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>20</v>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7">
         <f>3.69/100*4</f>
         <v>0.14760000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>23</v>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C8">
+        <f>26</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9">
+        <f>1.99/100*4</f>
+        <v>7.9600000000000004E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="4">
+        <v>14.63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="4"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12">
         <f>4/100*8</f>
         <v>0.32</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9">
-        <f>26</f>
+      <c r="D12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10">
-        <f>1.99/100*4</f>
-        <v>7.9600000000000004E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="4">
-        <v>14.63</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12">
+      <c r="B13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13">
         <f>2/10</f>
         <v>0.2</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="1"/>
-      <c r="C13"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="D13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="6"/>
+      <c r="B14" s="1"/>
+      <c r="C14"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C14"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="C15"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C15"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>0</v>
-      </c>
-      <c r="C16"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="B18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>1.76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C17">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="1" t="s">
+      <c r="C20">
+        <v>1.51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C18">
-        <v>1.76</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19">
-        <v>1.51</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20">
+      <c r="C21">
         <v>1.85</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C22"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C23"/>
@@ -667,10 +689,10 @@
       <c r="C29"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
       <c r="C30"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="1"/>
       <c r="C31"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -691,19 +713,22 @@
     <row r="37" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C37"/>
     </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C38"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B18" r:id="rId1"/>
-    <hyperlink ref="B20" r:id="rId2"/>
-    <hyperlink ref="B11" r:id="rId3"/>
-    <hyperlink ref="B10" r:id="rId4"/>
-    <hyperlink ref="B9" r:id="rId5"/>
-    <hyperlink ref="B19" r:id="rId6"/>
+    <hyperlink ref="B19" r:id="rId1"/>
+    <hyperlink ref="B21" r:id="rId2"/>
+    <hyperlink ref="B10" r:id="rId3"/>
+    <hyperlink ref="B9" r:id="rId4"/>
+    <hyperlink ref="B8" r:id="rId5"/>
+    <hyperlink ref="B20" r:id="rId6"/>
     <hyperlink ref="B6" r:id="rId7"/>
-    <hyperlink ref="B8" r:id="rId8"/>
-    <hyperlink ref="B17" r:id="rId9"/>
+    <hyperlink ref="B12" r:id="rId8"/>
+    <hyperlink ref="B18" r:id="rId9"/>
     <hyperlink ref="B5" r:id="rId10"/>
-    <hyperlink ref="B12" r:id="rId11"/>
+    <hyperlink ref="B13" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId12"/>

</xml_diff>